<commit_message>
Added elc details - % and values
</commit_message>
<xml_diff>
--- a/Data/raw_data/ELCs/elcs_en.xlsx
+++ b/Data/raw_data/ELCs/elcs_en.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PhD_Chapter1\Raw_data\ELCs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Data\raw_data\ELCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105F220A-944D-4439-AF59-1ADA7A5C140B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elcs_en" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">elcs_en!$A$1:$AC$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">elcs_en!$A$1:$AC$287</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6893" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6902" uniqueCount="1725">
   <si>
     <t>ogc_fid</t>
   </si>
@@ -5173,12 +5186,39 @@
   </si>
   <si>
     <t>Statistics_on_Cambodia_rubber_plantation_2013_MAFF__23.04.2014.pdf;Benh_Hoeurk_Kratie_Rubber_2_Company_Limited_in_MAFF_Statistic__08.06.2012.pdf</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>rubber</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Commodity value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producer value </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5656,10 +5696,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5980,16 +6024,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55:L84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6078,7 +6123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>287</v>
       </c>
@@ -6167,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>288</v>
       </c>
@@ -6256,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>289</v>
       </c>
@@ -6345,7 +6390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>290</v>
       </c>
@@ -6434,7 +6479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>291</v>
       </c>
@@ -6523,7 +6568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>292</v>
       </c>
@@ -6612,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>293</v>
       </c>
@@ -6701,7 +6746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>294</v>
       </c>
@@ -6790,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>295</v>
       </c>
@@ -6879,7 +6924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>296</v>
       </c>
@@ -6968,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>297</v>
       </c>
@@ -7057,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>298</v>
       </c>
@@ -7146,7 +7191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>299</v>
       </c>
@@ -7235,7 +7280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>300</v>
       </c>
@@ -7324,7 +7369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>301</v>
       </c>
@@ -7413,7 +7458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>302</v>
       </c>
@@ -7502,7 +7547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>303</v>
       </c>
@@ -7591,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>304</v>
       </c>
@@ -7680,7 +7725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>305</v>
       </c>
@@ -7769,7 +7814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>306</v>
       </c>
@@ -7858,7 +7903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>307</v>
       </c>
@@ -7947,7 +7992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>308</v>
       </c>
@@ -8036,7 +8081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>309</v>
       </c>
@@ -8125,7 +8170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>310</v>
       </c>
@@ -8214,7 +8259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>311</v>
       </c>
@@ -8303,7 +8348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>312</v>
       </c>
@@ -8392,7 +8437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>313</v>
       </c>
@@ -8481,7 +8526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>314</v>
       </c>
@@ -8570,7 +8615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>315</v>
       </c>
@@ -8659,7 +8704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>316</v>
       </c>
@@ -8748,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>317</v>
       </c>
@@ -8837,7 +8882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>318</v>
       </c>
@@ -8926,7 +8971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>319</v>
       </c>
@@ -9015,7 +9060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>320</v>
       </c>
@@ -9104,7 +9149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>321</v>
       </c>
@@ -9193,7 +9238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>322</v>
       </c>
@@ -9282,7 +9327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>323</v>
       </c>
@@ -9371,7 +9416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>324</v>
       </c>
@@ -9460,7 +9505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>325</v>
       </c>
@@ -9549,7 +9594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>326</v>
       </c>
@@ -9638,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>327</v>
       </c>
@@ -9727,7 +9772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>328</v>
       </c>
@@ -9816,7 +9861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>329</v>
       </c>
@@ -9905,7 +9950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>330</v>
       </c>
@@ -9994,7 +10039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>331</v>
       </c>
@@ -10083,7 +10128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>332</v>
       </c>
@@ -10172,7 +10217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>333</v>
       </c>
@@ -10261,7 +10306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>334</v>
       </c>
@@ -10350,7 +10395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>335</v>
       </c>
@@ -10439,7 +10484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>336</v>
       </c>
@@ -10528,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>337</v>
       </c>
@@ -10617,7 +10662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>338</v>
       </c>
@@ -10706,7 +10751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>339</v>
       </c>
@@ -10795,7 +10840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>340</v>
       </c>
@@ -10884,7 +10929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>341</v>
       </c>
@@ -10973,7 +11018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>342</v>
       </c>
@@ -11062,7 +11107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>343</v>
       </c>
@@ -11151,7 +11196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>344</v>
       </c>
@@ -11240,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>345</v>
       </c>
@@ -11329,7 +11374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>346</v>
       </c>
@@ -11418,7 +11463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>347</v>
       </c>
@@ -11507,7 +11552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>348</v>
       </c>
@@ -11596,7 +11641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>349</v>
       </c>
@@ -11685,7 +11730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>350</v>
       </c>
@@ -11774,7 +11819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>351</v>
       </c>
@@ -11863,7 +11908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>352</v>
       </c>
@@ -11952,7 +11997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>353</v>
       </c>
@@ -12041,7 +12086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>354</v>
       </c>
@@ -12130,7 +12175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>355</v>
       </c>
@@ -12219,7 +12264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>356</v>
       </c>
@@ -12308,7 +12353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>357</v>
       </c>
@@ -12397,7 +12442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>358</v>
       </c>
@@ -12486,7 +12531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>359</v>
       </c>
@@ -12575,7 +12620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>360</v>
       </c>
@@ -12664,7 +12709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>361</v>
       </c>
@@ -12753,7 +12798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>362</v>
       </c>
@@ -12842,7 +12887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>363</v>
       </c>
@@ -12931,7 +12976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>364</v>
       </c>
@@ -13020,7 +13065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>365</v>
       </c>
@@ -13109,7 +13154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>366</v>
       </c>
@@ -13198,7 +13243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>367</v>
       </c>
@@ -13287,7 +13332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>368</v>
       </c>
@@ -13376,7 +13421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>369</v>
       </c>
@@ -13465,7 +13510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>370</v>
       </c>
@@ -13554,7 +13599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>371</v>
       </c>
@@ -13643,7 +13688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>372</v>
       </c>
@@ -13732,7 +13777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>373</v>
       </c>
@@ -13821,7 +13866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>374</v>
       </c>
@@ -13910,7 +13955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>375</v>
       </c>
@@ -13999,7 +14044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>376</v>
       </c>
@@ -14088,7 +14133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>377</v>
       </c>
@@ -14177,7 +14222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>378</v>
       </c>
@@ -14266,7 +14311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>379</v>
       </c>
@@ -14355,7 +14400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>380</v>
       </c>
@@ -14444,7 +14489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>381</v>
       </c>
@@ -14533,7 +14578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>382</v>
       </c>
@@ -14622,7 +14667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>383</v>
       </c>
@@ -14711,7 +14756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>384</v>
       </c>
@@ -14800,7 +14845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>385</v>
       </c>
@@ -14889,7 +14934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>386</v>
       </c>
@@ -14978,7 +15023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>387</v>
       </c>
@@ -15067,7 +15112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>388</v>
       </c>
@@ -15156,7 +15201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>389</v>
       </c>
@@ -15245,7 +15290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>390</v>
       </c>
@@ -15334,7 +15379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>391</v>
       </c>
@@ -15423,7 +15468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>392</v>
       </c>
@@ -15512,7 +15557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>393</v>
       </c>
@@ -15601,7 +15646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>394</v>
       </c>
@@ -15690,7 +15735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>395</v>
       </c>
@@ -15779,7 +15824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>396</v>
       </c>
@@ -15868,7 +15913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>397</v>
       </c>
@@ -15957,7 +16002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>398</v>
       </c>
@@ -16046,7 +16091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>399</v>
       </c>
@@ -16135,7 +16180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>400</v>
       </c>
@@ -16224,7 +16269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>401</v>
       </c>
@@ -16313,7 +16358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>402</v>
       </c>
@@ -16402,7 +16447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>403</v>
       </c>
@@ -16491,7 +16536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>404</v>
       </c>
@@ -16580,7 +16625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>405</v>
       </c>
@@ -16669,7 +16714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>406</v>
       </c>
@@ -16758,7 +16803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>407</v>
       </c>
@@ -16847,7 +16892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>408</v>
       </c>
@@ -16936,7 +16981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>409</v>
       </c>
@@ -17025,7 +17070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>410</v>
       </c>
@@ -17114,7 +17159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>411</v>
       </c>
@@ -17203,7 +17248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>412</v>
       </c>
@@ -17292,7 +17337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>413</v>
       </c>
@@ -17381,7 +17426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>414</v>
       </c>
@@ -17470,7 +17515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>415</v>
       </c>
@@ -17559,7 +17604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>416</v>
       </c>
@@ -17648,7 +17693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>417</v>
       </c>
@@ -17737,7 +17782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>418</v>
       </c>
@@ -17826,7 +17871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>419</v>
       </c>
@@ -17915,7 +17960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>420</v>
       </c>
@@ -18004,7 +18049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>421</v>
       </c>
@@ -18093,7 +18138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>422</v>
       </c>
@@ -18182,7 +18227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>423</v>
       </c>
@@ -18271,7 +18316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>424</v>
       </c>
@@ -18360,7 +18405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>425</v>
       </c>
@@ -18449,7 +18494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>426</v>
       </c>
@@ -18538,7 +18583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>427</v>
       </c>
@@ -18627,7 +18672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>428</v>
       </c>
@@ -18716,7 +18761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>429</v>
       </c>
@@ -18805,7 +18850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>430</v>
       </c>
@@ -18894,7 +18939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>431</v>
       </c>
@@ -18983,7 +19028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>432</v>
       </c>
@@ -19072,7 +19117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>433</v>
       </c>
@@ -19161,7 +19206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>434</v>
       </c>
@@ -19250,7 +19295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>435</v>
       </c>
@@ -19339,7 +19384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>436</v>
       </c>
@@ -19428,7 +19473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>437</v>
       </c>
@@ -19517,7 +19562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>438</v>
       </c>
@@ -19606,7 +19651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>439</v>
       </c>
@@ -19695,7 +19740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>440</v>
       </c>
@@ -19784,7 +19829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>441</v>
       </c>
@@ -19873,7 +19918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>442</v>
       </c>
@@ -19962,7 +20007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>443</v>
       </c>
@@ -20051,7 +20096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>444</v>
       </c>
@@ -20140,7 +20185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>445</v>
       </c>
@@ -20229,7 +20274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>446</v>
       </c>
@@ -20318,7 +20363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>447</v>
       </c>
@@ -20407,7 +20452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>448</v>
       </c>
@@ -20496,7 +20541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>449</v>
       </c>
@@ -20585,7 +20630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>450</v>
       </c>
@@ -20674,7 +20719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>451</v>
       </c>
@@ -20763,7 +20808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>452</v>
       </c>
@@ -20852,7 +20897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>453</v>
       </c>
@@ -20941,7 +20986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>454</v>
       </c>
@@ -21030,7 +21075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>455</v>
       </c>
@@ -21119,7 +21164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>456</v>
       </c>
@@ -21208,7 +21253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>457</v>
       </c>
@@ -21297,7 +21342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>458</v>
       </c>
@@ -21386,7 +21431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>459</v>
       </c>
@@ -21475,7 +21520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>460</v>
       </c>
@@ -21564,7 +21609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>461</v>
       </c>
@@ -21653,7 +21698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>462</v>
       </c>
@@ -21742,7 +21787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>463</v>
       </c>
@@ -21831,7 +21876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>464</v>
       </c>
@@ -21920,7 +21965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>465</v>
       </c>
@@ -22009,7 +22054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>466</v>
       </c>
@@ -22098,7 +22143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>467</v>
       </c>
@@ -22187,7 +22232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>468</v>
       </c>
@@ -22276,7 +22321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>469</v>
       </c>
@@ -22365,7 +22410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>470</v>
       </c>
@@ -22454,7 +22499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>471</v>
       </c>
@@ -22543,7 +22588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>472</v>
       </c>
@@ -22632,7 +22677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>473</v>
       </c>
@@ -22721,7 +22766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>474</v>
       </c>
@@ -22810,7 +22855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>475</v>
       </c>
@@ -22899,7 +22944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>476</v>
       </c>
@@ -22988,7 +23033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>477</v>
       </c>
@@ -23077,7 +23122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>478</v>
       </c>
@@ -23166,7 +23211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>479</v>
       </c>
@@ -23255,7 +23300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>480</v>
       </c>
@@ -23344,7 +23389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>481</v>
       </c>
@@ -23433,7 +23478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>482</v>
       </c>
@@ -23522,7 +23567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>483</v>
       </c>
@@ -23611,7 +23656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>484</v>
       </c>
@@ -23700,7 +23745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>485</v>
       </c>
@@ -23789,7 +23834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>486</v>
       </c>
@@ -23878,7 +23923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>487</v>
       </c>
@@ -23967,7 +24012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>488</v>
       </c>
@@ -24056,7 +24101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>489</v>
       </c>
@@ -24145,7 +24190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>490</v>
       </c>
@@ -24234,7 +24279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>491</v>
       </c>
@@ -24323,7 +24368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>492</v>
       </c>
@@ -24412,7 +24457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>493</v>
       </c>
@@ -24501,7 +24546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>494</v>
       </c>
@@ -24590,7 +24635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>495</v>
       </c>
@@ -24679,7 +24724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>496</v>
       </c>
@@ -24768,7 +24813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>497</v>
       </c>
@@ -24857,7 +24902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>498</v>
       </c>
@@ -24946,7 +24991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>499</v>
       </c>
@@ -25035,7 +25080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>500</v>
       </c>
@@ -25124,7 +25169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>501</v>
       </c>
@@ -25213,7 +25258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>502</v>
       </c>
@@ -25302,7 +25347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>503</v>
       </c>
@@ -25391,7 +25436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>504</v>
       </c>
@@ -25480,7 +25525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>505</v>
       </c>
@@ -25569,7 +25614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>506</v>
       </c>
@@ -25658,7 +25703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>507</v>
       </c>
@@ -25747,7 +25792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>508</v>
       </c>
@@ -25836,7 +25881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>509</v>
       </c>
@@ -25925,7 +25970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>510</v>
       </c>
@@ -26014,7 +26059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>511</v>
       </c>
@@ -26103,7 +26148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>512</v>
       </c>
@@ -26192,7 +26237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>513</v>
       </c>
@@ -26281,7 +26326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>514</v>
       </c>
@@ -26370,7 +26415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>515</v>
       </c>
@@ -26459,7 +26504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>516</v>
       </c>
@@ -26548,7 +26593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>517</v>
       </c>
@@ -26637,7 +26682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>518</v>
       </c>
@@ -26726,7 +26771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>519</v>
       </c>
@@ -26815,7 +26860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>520</v>
       </c>
@@ -26904,7 +26949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>521</v>
       </c>
@@ -26993,7 +27038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>522</v>
       </c>
@@ -27082,7 +27127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>523</v>
       </c>
@@ -27171,7 +27216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>524</v>
       </c>
@@ -27260,7 +27305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>525</v>
       </c>
@@ -27349,7 +27394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>526</v>
       </c>
@@ -27438,7 +27483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>527</v>
       </c>
@@ -27527,7 +27572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>528</v>
       </c>
@@ -27616,7 +27661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>529</v>
       </c>
@@ -27705,7 +27750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>530</v>
       </c>
@@ -27794,7 +27839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>531</v>
       </c>
@@ -27883,7 +27928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>532</v>
       </c>
@@ -27972,7 +28017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>533</v>
       </c>
@@ -28061,7 +28106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>534</v>
       </c>
@@ -28150,7 +28195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>535</v>
       </c>
@@ -28239,7 +28284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>536</v>
       </c>
@@ -28328,7 +28373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>537</v>
       </c>
@@ -28417,7 +28462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>538</v>
       </c>
@@ -28506,7 +28551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>539</v>
       </c>
@@ -28595,7 +28640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>540</v>
       </c>
@@ -28684,7 +28729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>541</v>
       </c>
@@ -28773,7 +28818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>542</v>
       </c>
@@ -28862,7 +28907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>543</v>
       </c>
@@ -28951,7 +28996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>544</v>
       </c>
@@ -29040,7 +29085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>545</v>
       </c>
@@ -29129,7 +29174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>546</v>
       </c>
@@ -29218,7 +29263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>547</v>
       </c>
@@ -29307,7 +29352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>548</v>
       </c>
@@ -29396,7 +29441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>549</v>
       </c>
@@ -29485,7 +29530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>550</v>
       </c>
@@ -29574,7 +29619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>551</v>
       </c>
@@ -29663,7 +29708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>552</v>
       </c>
@@ -29752,7 +29797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>553</v>
       </c>
@@ -29841,7 +29886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>554</v>
       </c>
@@ -29930,7 +29975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>555</v>
       </c>
@@ -30019,7 +30064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>556</v>
       </c>
@@ -30108,7 +30153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>557</v>
       </c>
@@ -30197,7 +30242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>558</v>
       </c>
@@ -30286,7 +30331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>559</v>
       </c>
@@ -30375,7 +30420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>560</v>
       </c>
@@ -30464,7 +30509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>561</v>
       </c>
@@ -30553,7 +30598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>562</v>
       </c>
@@ -30642,7 +30687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>563</v>
       </c>
@@ -30731,7 +30776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>564</v>
       </c>
@@ -30820,7 +30865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>565</v>
       </c>
@@ -30909,7 +30954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>566</v>
       </c>
@@ -30998,7 +31043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>567</v>
       </c>
@@ -31087,7 +31132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>568</v>
       </c>
@@ -31176,7 +31221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>569</v>
       </c>
@@ -31265,7 +31310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>570</v>
       </c>
@@ -31354,7 +31399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>571</v>
       </c>
@@ -31443,7 +31488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>572</v>
       </c>
@@ -31533,7 +31578,140 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC1"/>
+  <autoFilter ref="A1:AC287" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Peanut;Rice;Corn;Soybean;Other crops;Animal husbandry"/>
+        <filter val="Rice"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2853456E-D63E-42EC-8552-5A59930970D9}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B1">
+        <v>287</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1722</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B2">
+        <v>147</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/$B$1*100</f>
+        <v>51.219512195121951</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C6" si="0">B3/$B$1*100</f>
+        <v>8.0139372822299642</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7421602787456445</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.69686411149825789</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B6">
+    <sortCondition descending="1" ref="B1:B6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edited ELC summary table. Now included in SI
</commit_message>
<xml_diff>
--- a/Data/raw_data/ELCs/elcs_en.xlsx
+++ b/Data/raw_data/ELCs/elcs_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Data\raw_data\ELCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105F220A-944D-4439-AF59-1ADA7A5C140B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9955E30-087C-49FC-9A45-301E47B90B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elcs_en" sheetId="1" r:id="rId1"/>
@@ -6025,14 +6025,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC287"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55:L84"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -6123,7 +6125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>287</v>
       </c>
@@ -6212,7 +6214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>288</v>
       </c>
@@ -6301,7 +6303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>289</v>
       </c>
@@ -6390,7 +6392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>290</v>
       </c>
@@ -6479,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>291</v>
       </c>
@@ -6568,7 +6570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>292</v>
       </c>
@@ -6657,7 +6659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>293</v>
       </c>
@@ -6746,7 +6748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>294</v>
       </c>
@@ -6835,7 +6837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>295</v>
       </c>
@@ -6924,7 +6926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>296</v>
       </c>
@@ -7013,7 +7015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>297</v>
       </c>
@@ -7102,7 +7104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>298</v>
       </c>
@@ -7191,7 +7193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>299</v>
       </c>
@@ -7280,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>300</v>
       </c>
@@ -7369,7 +7371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>301</v>
       </c>
@@ -7458,7 +7460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>302</v>
       </c>
@@ -7547,7 +7549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>303</v>
       </c>
@@ -7636,7 +7638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>304</v>
       </c>
@@ -7725,7 +7727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>305</v>
       </c>
@@ -7814,7 +7816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>306</v>
       </c>
@@ -7903,7 +7905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>307</v>
       </c>
@@ -7992,7 +7994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>308</v>
       </c>
@@ -8081,7 +8083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>309</v>
       </c>
@@ -8170,7 +8172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>310</v>
       </c>
@@ -8259,7 +8261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>311</v>
       </c>
@@ -8348,7 +8350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>312</v>
       </c>
@@ -8437,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>313</v>
       </c>
@@ -8526,7 +8528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>314</v>
       </c>
@@ -8615,7 +8617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>315</v>
       </c>
@@ -8704,7 +8706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>316</v>
       </c>
@@ -8793,7 +8795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>317</v>
       </c>
@@ -8882,7 +8884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>318</v>
       </c>
@@ -8971,7 +8973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>319</v>
       </c>
@@ -9060,7 +9062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>320</v>
       </c>
@@ -9149,7 +9151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>321</v>
       </c>
@@ -9238,7 +9240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>322</v>
       </c>
@@ -9327,7 +9329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>323</v>
       </c>
@@ -9416,7 +9418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>324</v>
       </c>
@@ -9505,7 +9507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>325</v>
       </c>
@@ -9594,7 +9596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>326</v>
       </c>
@@ -9683,7 +9685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>327</v>
       </c>
@@ -9772,7 +9774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>328</v>
       </c>
@@ -9861,7 +9863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>329</v>
       </c>
@@ -9950,7 +9952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>330</v>
       </c>
@@ -10039,7 +10041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>331</v>
       </c>
@@ -10128,7 +10130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>332</v>
       </c>
@@ -10217,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>333</v>
       </c>
@@ -10306,7 +10308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>334</v>
       </c>
@@ -10395,7 +10397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>335</v>
       </c>
@@ -10484,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>336</v>
       </c>
@@ -10573,7 +10575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>337</v>
       </c>
@@ -10662,7 +10664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>338</v>
       </c>
@@ -10751,7 +10753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>339</v>
       </c>
@@ -11196,7 +11198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>344</v>
       </c>
@@ -11285,7 +11287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>345</v>
       </c>
@@ -11374,7 +11376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>346</v>
       </c>
@@ -11463,7 +11465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>347</v>
       </c>
@@ -11552,7 +11554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>348</v>
       </c>
@@ -11641,7 +11643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>349</v>
       </c>
@@ -11730,7 +11732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>350</v>
       </c>
@@ -11819,7 +11821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>351</v>
       </c>
@@ -11908,7 +11910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>352</v>
       </c>
@@ -11997,7 +11999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>353</v>
       </c>
@@ -12086,7 +12088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>354</v>
       </c>
@@ -12175,7 +12177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>355</v>
       </c>
@@ -12264,7 +12266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>356</v>
       </c>
@@ -12353,7 +12355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>357</v>
       </c>
@@ -12442,7 +12444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>358</v>
       </c>
@@ -12531,7 +12533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>359</v>
       </c>
@@ -12620,7 +12622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>360</v>
       </c>
@@ -12709,7 +12711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>361</v>
       </c>
@@ -12798,7 +12800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>362</v>
       </c>
@@ -12887,7 +12889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>363</v>
       </c>
@@ -12976,7 +12978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>364</v>
       </c>
@@ -13065,7 +13067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>365</v>
       </c>
@@ -13154,7 +13156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>366</v>
       </c>
@@ -13243,7 +13245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>367</v>
       </c>
@@ -13332,7 +13334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>368</v>
       </c>
@@ -13510,7 +13512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>370</v>
       </c>
@@ -13599,7 +13601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>371</v>
       </c>
@@ -13688,7 +13690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>372</v>
       </c>
@@ -13777,7 +13779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>373</v>
       </c>
@@ -13866,7 +13868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>374</v>
       </c>
@@ -13955,7 +13957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>375</v>
       </c>
@@ -14044,7 +14046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>376</v>
       </c>
@@ -14133,7 +14135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>377</v>
       </c>
@@ -14222,7 +14224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>378</v>
       </c>
@@ -14311,7 +14313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>379</v>
       </c>
@@ -14400,7 +14402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>380</v>
       </c>
@@ -14489,7 +14491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>381</v>
       </c>
@@ -14578,7 +14580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>382</v>
       </c>
@@ -14667,7 +14669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>383</v>
       </c>
@@ -14756,7 +14758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>384</v>
       </c>
@@ -14845,7 +14847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>385</v>
       </c>
@@ -14934,7 +14936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>386</v>
       </c>
@@ -15023,7 +15025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>387</v>
       </c>
@@ -15112,7 +15114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>388</v>
       </c>
@@ -15201,7 +15203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>389</v>
       </c>
@@ -15290,7 +15292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>390</v>
       </c>
@@ -15379,7 +15381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>391</v>
       </c>
@@ -15468,7 +15470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>392</v>
       </c>
@@ -15557,7 +15559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>393</v>
       </c>
@@ -15646,7 +15648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>394</v>
       </c>
@@ -15735,7 +15737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>395</v>
       </c>
@@ -15824,7 +15826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>396</v>
       </c>
@@ -15913,7 +15915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>397</v>
       </c>
@@ -16002,7 +16004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>398</v>
       </c>
@@ -16091,7 +16093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>399</v>
       </c>
@@ -16180,7 +16182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>400</v>
       </c>
@@ -16269,7 +16271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>401</v>
       </c>
@@ -16358,7 +16360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>402</v>
       </c>
@@ -16447,7 +16449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>403</v>
       </c>
@@ -16536,7 +16538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>404</v>
       </c>
@@ -16625,7 +16627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>405</v>
       </c>
@@ -16714,7 +16716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>406</v>
       </c>
@@ -16803,7 +16805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>407</v>
       </c>
@@ -16892,7 +16894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>408</v>
       </c>
@@ -16981,7 +16983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>409</v>
       </c>
@@ -17070,7 +17072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>410</v>
       </c>
@@ -17159,7 +17161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>411</v>
       </c>
@@ -17248,7 +17250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>412</v>
       </c>
@@ -17337,7 +17339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>413</v>
       </c>
@@ -17426,7 +17428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>414</v>
       </c>
@@ -17515,7 +17517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>415</v>
       </c>
@@ -17604,7 +17606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>416</v>
       </c>
@@ -17693,7 +17695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>417</v>
       </c>
@@ -17782,7 +17784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>418</v>
       </c>
@@ -17871,7 +17873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>419</v>
       </c>
@@ -17960,7 +17962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>420</v>
       </c>
@@ -18049,7 +18051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>421</v>
       </c>
@@ -18138,7 +18140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>422</v>
       </c>
@@ -18227,7 +18229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>423</v>
       </c>
@@ -18316,7 +18318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>424</v>
       </c>
@@ -18405,7 +18407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>425</v>
       </c>
@@ -18494,7 +18496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>426</v>
       </c>
@@ -18583,7 +18585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>427</v>
       </c>
@@ -18672,7 +18674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>428</v>
       </c>
@@ -18761,7 +18763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>429</v>
       </c>
@@ -18850,7 +18852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>430</v>
       </c>
@@ -18939,7 +18941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>431</v>
       </c>
@@ -19028,7 +19030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>432</v>
       </c>
@@ -19117,7 +19119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>433</v>
       </c>
@@ -19206,7 +19208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>434</v>
       </c>
@@ -19295,7 +19297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>435</v>
       </c>
@@ -19384,7 +19386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>436</v>
       </c>
@@ -19473,7 +19475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>437</v>
       </c>
@@ -19562,7 +19564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>438</v>
       </c>
@@ -19651,7 +19653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>439</v>
       </c>
@@ -19740,7 +19742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>440</v>
       </c>
@@ -19829,7 +19831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>441</v>
       </c>
@@ -19918,7 +19920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>442</v>
       </c>
@@ -20007,7 +20009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>443</v>
       </c>
@@ -20096,7 +20098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>444</v>
       </c>
@@ -20185,7 +20187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>445</v>
       </c>
@@ -20274,7 +20276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>446</v>
       </c>
@@ -20363,7 +20365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>447</v>
       </c>
@@ -20452,7 +20454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>448</v>
       </c>
@@ -20541,7 +20543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>449</v>
       </c>
@@ -20630,7 +20632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>450</v>
       </c>
@@ -20719,7 +20721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>451</v>
       </c>
@@ -20808,7 +20810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>452</v>
       </c>
@@ -20897,7 +20899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>453</v>
       </c>
@@ -20986,7 +20988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>454</v>
       </c>
@@ -21075,7 +21077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>455</v>
       </c>
@@ -21164,7 +21166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>456</v>
       </c>
@@ -21253,7 +21255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>457</v>
       </c>
@@ -21342,7 +21344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>458</v>
       </c>
@@ -21431,7 +21433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>459</v>
       </c>
@@ -21520,7 +21522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>460</v>
       </c>
@@ -21609,7 +21611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>461</v>
       </c>
@@ -21698,7 +21700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>462</v>
       </c>
@@ -21787,7 +21789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>463</v>
       </c>
@@ -21876,7 +21878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>464</v>
       </c>
@@ -21965,7 +21967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>465</v>
       </c>
@@ -22054,7 +22056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>466</v>
       </c>
@@ -22143,7 +22145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>467</v>
       </c>
@@ -22232,7 +22234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>468</v>
       </c>
@@ -22321,7 +22323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>469</v>
       </c>
@@ -22410,7 +22412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>470</v>
       </c>
@@ -22499,7 +22501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>471</v>
       </c>
@@ -22588,7 +22590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>472</v>
       </c>
@@ -22677,7 +22679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>473</v>
       </c>
@@ -22766,7 +22768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>474</v>
       </c>
@@ -22855,7 +22857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>475</v>
       </c>
@@ -22944,7 +22946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>476</v>
       </c>
@@ -23033,7 +23035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>477</v>
       </c>
@@ -23122,7 +23124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>478</v>
       </c>
@@ -23211,7 +23213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>479</v>
       </c>
@@ -23300,7 +23302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>480</v>
       </c>
@@ -23389,7 +23391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>481</v>
       </c>
@@ -23478,7 +23480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>482</v>
       </c>
@@ -23567,7 +23569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>483</v>
       </c>
@@ -23656,7 +23658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>484</v>
       </c>
@@ -23745,7 +23747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>485</v>
       </c>
@@ -23834,7 +23836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>486</v>
       </c>
@@ -23923,7 +23925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>487</v>
       </c>
@@ -24012,7 +24014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>488</v>
       </c>
@@ -24101,7 +24103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>489</v>
       </c>
@@ -24190,7 +24192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>490</v>
       </c>
@@ -24279,7 +24281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>491</v>
       </c>
@@ -24368,7 +24370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>492</v>
       </c>
@@ -24457,7 +24459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>493</v>
       </c>
@@ -24546,7 +24548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>494</v>
       </c>
@@ -24635,7 +24637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>495</v>
       </c>
@@ -24724,7 +24726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>496</v>
       </c>
@@ -24813,7 +24815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>497</v>
       </c>
@@ -24902,7 +24904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>498</v>
       </c>
@@ -24991,7 +24993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>499</v>
       </c>
@@ -25080,7 +25082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>500</v>
       </c>
@@ -25169,7 +25171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>501</v>
       </c>
@@ -25258,7 +25260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>502</v>
       </c>
@@ -25347,7 +25349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>503</v>
       </c>
@@ -25436,7 +25438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>504</v>
       </c>
@@ -25525,7 +25527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>505</v>
       </c>
@@ -25614,7 +25616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>506</v>
       </c>
@@ -25703,7 +25705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>507</v>
       </c>
@@ -25792,7 +25794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>508</v>
       </c>
@@ -25881,7 +25883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>509</v>
       </c>
@@ -25970,7 +25972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>510</v>
       </c>
@@ -26059,7 +26061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>511</v>
       </c>
@@ -26148,7 +26150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>512</v>
       </c>
@@ -26237,7 +26239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>513</v>
       </c>
@@ -26326,7 +26328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>514</v>
       </c>
@@ -26415,7 +26417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>515</v>
       </c>
@@ -26504,7 +26506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>516</v>
       </c>
@@ -26593,7 +26595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>517</v>
       </c>
@@ -26682,7 +26684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>518</v>
       </c>
@@ -26771,7 +26773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>519</v>
       </c>
@@ -26860,7 +26862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>520</v>
       </c>
@@ -26949,7 +26951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>521</v>
       </c>
@@ -27038,7 +27040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>522</v>
       </c>
@@ -27127,7 +27129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>523</v>
       </c>
@@ -27216,7 +27218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>524</v>
       </c>
@@ -27305,7 +27307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>525</v>
       </c>
@@ -27394,7 +27396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>526</v>
       </c>
@@ -27483,7 +27485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>527</v>
       </c>
@@ -27572,7 +27574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>528</v>
       </c>
@@ -27661,7 +27663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>529</v>
       </c>
@@ -27750,7 +27752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>530</v>
       </c>
@@ -27839,7 +27841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>531</v>
       </c>
@@ -27928,7 +27930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>532</v>
       </c>
@@ -28017,7 +28019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>533</v>
       </c>
@@ -28106,7 +28108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>534</v>
       </c>
@@ -28195,7 +28197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>535</v>
       </c>
@@ -28284,7 +28286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>536</v>
       </c>
@@ -28373,7 +28375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>537</v>
       </c>
@@ -28462,7 +28464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>538</v>
       </c>
@@ -28551,7 +28553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>539</v>
       </c>
@@ -28640,7 +28642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>540</v>
       </c>
@@ -28729,7 +28731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>541</v>
       </c>
@@ -28818,7 +28820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>542</v>
       </c>
@@ -28907,7 +28909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>543</v>
       </c>
@@ -28996,7 +28998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>544</v>
       </c>
@@ -29085,7 +29087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>545</v>
       </c>
@@ -29174,7 +29176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>546</v>
       </c>
@@ -29263,7 +29265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>547</v>
       </c>
@@ -29352,7 +29354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>548</v>
       </c>
@@ -29441,7 +29443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>549</v>
       </c>
@@ -29530,7 +29532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>550</v>
       </c>
@@ -29619,7 +29621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>551</v>
       </c>
@@ -29708,7 +29710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>552</v>
       </c>
@@ -29797,7 +29799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>553</v>
       </c>
@@ -29886,7 +29888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>554</v>
       </c>
@@ -29975,7 +29977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>555</v>
       </c>
@@ -30064,7 +30066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>556</v>
       </c>
@@ -30153,7 +30155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>557</v>
       </c>
@@ -30242,7 +30244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>558</v>
       </c>
@@ -30331,7 +30333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>559</v>
       </c>
@@ -30420,7 +30422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>560</v>
       </c>
@@ -30509,7 +30511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>561</v>
       </c>
@@ -30598,7 +30600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>562</v>
       </c>
@@ -30687,7 +30689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>563</v>
       </c>
@@ -30776,7 +30778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>564</v>
       </c>
@@ -30865,7 +30867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>565</v>
       </c>
@@ -30954,7 +30956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>566</v>
       </c>
@@ -31043,7 +31045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>567</v>
       </c>
@@ -31132,7 +31134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>568</v>
       </c>
@@ -31221,7 +31223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>569</v>
       </c>
@@ -31310,7 +31312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>570</v>
       </c>
@@ -31399,7 +31401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>571</v>
       </c>
@@ -31488,7 +31490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>572</v>
       </c>
@@ -31578,14 +31580,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC287" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="Peanut;Rice;Corn;Soybean;Other crops;Animal husbandry"/>
-        <filter val="Rice"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC287" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -31595,7 +31590,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>